<commit_message>
0.0.8: finish method implemented. it will be called before return to micronaut.
</commit_message>
<xml_diff>
--- a/meta/telegrams/HttpCommonRequest.xlsx
+++ b/meta/telegrams/HttpCommonRequest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/telegrams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/cacco/oplux/oplux-v3-api-common/blanco-meta/value-object/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EF4D33-3315-CB4A-B1F2-8A114A28632A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AC5F92-4969-DE4D-9AD3-33C167E300C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23440" yWindow="19700" windowWidth="25020" windowHeight="11540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>クラス名</t>
   </si>
@@ -513,6 +513,50 @@
     </rPh>
     <rPh sb="4" eb="6">
       <t xml:space="preserve">ヘンスウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>noAuthentication</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>metaIdList</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>List</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>認証が不要なAPIであればtrue</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンショウガ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">フヨウナ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>メタID情報（文字列）のリスト</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ジョウホウ </t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t xml:space="preserve">モジレツ </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1651,46 +1695,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1706,14 +1711,53 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2126,10 +2170,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:W63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G39" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2260,10 +2304,10 @@
       <c r="F9" s="84"/>
     </row>
     <row r="10" spans="1:21" s="31" customFormat="1">
-      <c r="A10" s="98" t="s">
+      <c r="A10" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="99"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="70" t="s">
         <v>49</v>
       </c>
@@ -2667,7 +2711,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="110"/>
+      <c r="E28" s="98"/>
       <c r="F28" s="77"/>
       <c r="N28" s="77"/>
       <c r="O28" s="77"/>
@@ -2679,19 +2723,19 @@
       <c r="U28" s="77"/>
     </row>
     <row r="29" spans="1:21" s="31" customFormat="1">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="104" t="s">
+      <c r="D29" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="111" t="s">
+      <c r="E29" s="121" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="80"/>
@@ -2711,11 +2755,11 @@
       <c r="U29" s="77"/>
     </row>
     <row r="30" spans="1:21" s="31" customFormat="1">
-      <c r="A30" s="105"/>
-      <c r="B30" s="105"/>
-      <c r="C30" s="104"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="111"/>
+      <c r="A30" s="114"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="121"/>
       <c r="F30" s="80"/>
       <c r="G30" s="73"/>
       <c r="H30" s="73"/>
@@ -2745,7 +2789,7 @@
       <c r="D31" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="112" t="s">
+      <c r="E31" s="99" t="s">
         <v>73</v>
       </c>
       <c r="F31" s="80"/>
@@ -2770,7 +2814,7 @@
       <c r="B32" s="17"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="112"/>
+      <c r="E32" s="99"/>
       <c r="F32" s="80"/>
       <c r="G32" s="73"/>
       <c r="H32" s="73"/>
@@ -2793,7 +2837,7 @@
       <c r="B33" s="17"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="112"/>
+      <c r="E33" s="99"/>
       <c r="F33" s="80"/>
       <c r="G33" s="73"/>
       <c r="H33" s="73"/>
@@ -2816,7 +2860,7 @@
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="112"/>
+      <c r="E34" s="99"/>
       <c r="F34" s="80"/>
       <c r="G34" s="73"/>
       <c r="H34" s="73"/>
@@ -2839,7 +2883,7 @@
       <c r="B35" s="17"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="112"/>
+      <c r="E35" s="99"/>
       <c r="F35" s="80"/>
       <c r="G35" s="73"/>
       <c r="H35" s="73"/>
@@ -2858,11 +2902,11 @@
       <c r="U35" s="77"/>
     </row>
     <row r="36" spans="1:23" s="31" customFormat="1">
-      <c r="A36" s="113"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="116"/>
+      <c r="A36" s="100"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="103"/>
       <c r="F36" s="80"/>
       <c r="G36" s="73"/>
       <c r="H36" s="73"/>
@@ -3069,78 +3113,78 @@
       <c r="W44" s="12"/>
     </row>
     <row r="45" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="104" t="s">
+      <c r="C45" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="104" t="s">
+      <c r="D45" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="106" t="s">
+      <c r="E45" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="104" t="s">
+      <c r="F45" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="104" t="s">
+      <c r="G45" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="H45" s="104" t="s">
+      <c r="H45" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="I45" s="104" t="s">
+      <c r="I45" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="J45" s="100" t="s">
+      <c r="J45" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="K45" s="100" t="s">
+      <c r="K45" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="L45" s="119" t="s">
+      <c r="L45" s="109" t="s">
         <v>80</v>
       </c>
-      <c r="M45" s="108" t="s">
+      <c r="M45" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="N45" s="102" t="s">
+      <c r="N45" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="O45" s="103"/>
-      <c r="P45" s="102" t="s">
+      <c r="O45" s="112"/>
+      <c r="P45" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="Q45" s="103"/>
+      <c r="Q45" s="112"/>
       <c r="R45" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="S45" s="104" t="s">
+      <c r="S45" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="T45" s="104"/>
+      <c r="T45" s="113"/>
       <c r="U45" s="13"/>
       <c r="V45" s="14"/>
       <c r="W45" s="7"/>
     </row>
     <row r="46" spans="1:23">
-      <c r="A46" s="105"/>
-      <c r="B46" s="105"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="104"/>
-      <c r="E46" s="107"/>
-      <c r="F46" s="104"/>
-      <c r="G46" s="104"/>
-      <c r="H46" s="104"/>
-      <c r="I46" s="104"/>
-      <c r="J46" s="101"/>
-      <c r="K46" s="101"/>
-      <c r="L46" s="120"/>
-      <c r="M46" s="109"/>
+      <c r="A46" s="114"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="113"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="113"/>
+      <c r="H46" s="113"/>
+      <c r="I46" s="113"/>
+      <c r="J46" s="118"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="110"/>
+      <c r="M46" s="120"/>
       <c r="N46" s="38" t="s">
         <v>14</v>
       </c>
@@ -3156,8 +3200,8 @@
       <c r="R46" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="S46" s="104"/>
-      <c r="T46" s="104"/>
+      <c r="S46" s="113"/>
+      <c r="T46" s="113"/>
       <c r="U46" s="15"/>
       <c r="V46" s="27"/>
       <c r="W46" s="12"/>
@@ -3181,11 +3225,11 @@
       <c r="H47" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="I47" s="117" t="s">
+      <c r="I47" s="104" t="s">
         <v>74</v>
       </c>
       <c r="J47" s="90"/>
-      <c r="K47" s="121"/>
+      <c r="K47" s="106"/>
       <c r="L47" s="86" t="s">
         <v>38</v>
       </c>
@@ -3207,28 +3251,25 @@
     </row>
     <row r="48" spans="1:23" ht="15">
       <c r="A48" s="16">
+        <f>A47+1</f>
         <v>2</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="G48" s="18"/>
       <c r="H48" s="18"/>
-      <c r="I48" s="118" t="s">
+      <c r="I48" s="105" t="s">
         <v>66</v>
       </c>
       <c r="J48" s="18"/>
-      <c r="K48" s="87" t="s">
-        <v>38</v>
-      </c>
+      <c r="K48" s="87"/>
       <c r="L48" s="87" t="s">
         <v>38</v>
       </c>
@@ -3241,58 +3282,98 @@
       <c r="Q48" s="18"/>
       <c r="R48" s="18"/>
       <c r="S48" s="18" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="T48" s="19"/>
       <c r="U48" s="19"/>
       <c r="V48" s="20"/>
       <c r="W48" s="12"/>
     </row>
-    <row r="49" spans="1:23">
-      <c r="A49" s="16"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
+    <row r="49" spans="1:23" ht="15">
+      <c r="A49" s="16">
+        <f t="shared" ref="A49:A50" si="0">A48+1</f>
+        <v>3</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="G49" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I49" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="J49" s="18"/>
-      <c r="K49" s="87"/>
-      <c r="L49" s="87"/>
-      <c r="M49" s="87"/>
+      <c r="K49" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="M49" s="87" t="s">
+        <v>38</v>
+      </c>
       <c r="N49" s="18"/>
       <c r="O49" s="18"/>
       <c r="P49" s="18"/>
       <c r="Q49" s="18"/>
       <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
+      <c r="S49" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="T49" s="19"/>
       <c r="U49" s="19"/>
       <c r="V49" s="20"/>
       <c r="W49" s="12"/>
     </row>
-    <row r="50" spans="1:23">
-      <c r="A50" s="16"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+    <row r="50" spans="1:23" ht="15">
+      <c r="A50" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>60</v>
+      </c>
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="I50" s="105" t="s">
+        <v>66</v>
+      </c>
       <c r="J50" s="18"/>
-      <c r="K50" s="87"/>
-      <c r="L50" s="87"/>
-      <c r="M50" s="87"/>
+      <c r="K50" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="L50" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="M50" s="87" t="s">
+        <v>38</v>
+      </c>
       <c r="N50" s="18"/>
       <c r="O50" s="18"/>
       <c r="P50" s="18"/>
       <c r="Q50" s="18"/>
       <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
+      <c r="S50" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="T50" s="19"/>
       <c r="U50" s="19"/>
       <c r="V50" s="20"/>
@@ -3304,19 +3385,19 @@
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="88"/>
-      <c r="L51" s="88"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="87"/>
+      <c r="L51" s="87"/>
       <c r="M51" s="87"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="42"/>
-      <c r="P51" s="42"/>
-      <c r="Q51" s="42"/>
-      <c r="R51" s="42"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
       <c r="S51" s="18"/>
       <c r="T51" s="19"/>
       <c r="U51" s="19"/>
@@ -3454,19 +3535,19 @@
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="87"/>
-      <c r="L57" s="87"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="88"/>
+      <c r="L57" s="88"/>
       <c r="M57" s="87"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
+      <c r="N57" s="42"/>
+      <c r="O57" s="42"/>
+      <c r="P57" s="42"/>
+      <c r="Q57" s="42"/>
+      <c r="R57" s="42"/>
       <c r="S57" s="18"/>
       <c r="T57" s="19"/>
       <c r="U57" s="19"/>
@@ -3549,29 +3630,79 @@
       <c r="W60" s="12"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="21"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="G61" s="23"/>
-      <c r="H61" s="23"/>
-      <c r="I61" s="23"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="89"/>
-      <c r="L61" s="89"/>
-      <c r="M61" s="96"/>
-      <c r="N61" s="23"/>
-      <c r="O61" s="23"/>
-      <c r="P61" s="23"/>
-      <c r="Q61" s="23"/>
-      <c r="R61" s="23"/>
-      <c r="S61" s="23"/>
-      <c r="T61" s="24"/>
-      <c r="U61" s="24"/>
-      <c r="V61" s="25"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="87"/>
+      <c r="L61" s="87"/>
+      <c r="M61" s="87"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="19"/>
+      <c r="U61" s="19"/>
+      <c r="V61" s="20"/>
       <c r="W61" s="12"/>
+    </row>
+    <row r="62" spans="1:23">
+      <c r="A62" s="16"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="87"/>
+      <c r="L62" s="87"/>
+      <c r="M62" s="87"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
+      <c r="S62" s="18"/>
+      <c r="T62" s="19"/>
+      <c r="U62" s="19"/>
+      <c r="V62" s="20"/>
+      <c r="W62" s="12"/>
+    </row>
+    <row r="63" spans="1:23">
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="89"/>
+      <c r="L63" s="89"/>
+      <c r="M63" s="96"/>
+      <c r="N63" s="23"/>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23"/>
+      <c r="Q63" s="23"/>
+      <c r="R63" s="23"/>
+      <c r="S63" s="23"/>
+      <c r="T63" s="24"/>
+      <c r="U63" s="24"/>
+      <c r="V63" s="25"/>
+      <c r="W63" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -3599,8 +3730,8 @@
     <mergeCell ref="H45:H46"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="10">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N67:R67 F77 M72" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N69:R69 F79 M74" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3612,9 +3743,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{C21BA24C-69B4-FA48-BE39-8BC5867C6E31}">
       <formula1>adjustDefaultValue</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L47:L61" xr:uid="{BF4683B4-0915-0242-997D-7FB58A59D5DA}">
-      <formula1>theOther</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{5E1FE143-8BD9-EB43-A8F8-EBFA0B3D612E}">
       <formula1>accessScope</formula1>
@@ -3628,7 +3756,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{2FED42AB-6D5F-2840-8FD3-655E06727165}">
       <formula1>isData</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K47:K61" xr:uid="{90D0A52A-15A4-0748-B78D-220B9183D38D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K47:M63" xr:uid="{BF4683B4-0915-0242-997D-7FB58A59D5DA}">
       <formula1>theOther</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>